<commit_message>
Able to flatten parts and assemblies
</commit_message>
<xml_diff>
--- a/01-EL-001.xlsx
+++ b/01-EL-001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Isaac python\BOMManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{62F7B8B4-6085-4666-B78F-E7A8257A1980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{339E5259-3119-412A-A356-3548C2CE3187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12615" windowWidth="16440" windowHeight="28320" xr2:uid="{D6E755FC-5AB3-408D-BD54-FB688D436BF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D6E755FC-5AB3-408D-BD54-FB688D436BF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -296,12 +296,24 @@
       <name val="SWGDT"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -316,11 +328,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,13 +359,18 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0013ACFC-0E87-450B-92BB-FF76B25836EB}" diskRevisions="1" revisionId="31" version="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{CC6B5E40-B788-4D99-9FC6-BE31FE63855C}" diskRevisions="1" revisionId="31" version="3">
   <header guid="{CA8955DD-9B4C-48B9-8E3B-7F4841ADBFD5}" dateTime="2022-06-13T15:38:32" maxSheetId="2" userName="Isaac" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
   <header guid="{0013ACFC-0E87-450B-92BB-FF76B25836EB}" dateTime="2022-06-13T15:40:09" maxSheetId="2" userName="Isaac" r:id="rId2" minRId="1" maxRId="31">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CC6B5E40-B788-4D99-9FC6-BE31FE63855C}" dateTime="2022-06-16T15:32:36" maxSheetId="2" userName="Isaac" r:id="rId3">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -602,7 +627,255 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="1" sqref="A2:XFD2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A3:XFD7">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A21:XFD21">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A8:XFD8">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A28:XFD28">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A9:XFD9">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A10:XFD10">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A11:XFD11">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A2:XFD11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="B10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A2:XFD11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A12:XFD12">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A13:XFD13">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A14:XFD14">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A15:XFD15">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A16:XFD16">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A17:XFD17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A18:XFD18">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A19:XFD19">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A20:XFD20">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A22:XFD22">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A23:XFD23">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A24:XFD24">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A25:XFD25">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A26:XFD26">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A27:XFD27">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="1" sqref="A29:XFD29">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
@@ -905,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AC3A761-772A-43E9-ACC9-14704B31FCAA}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A30:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -930,395 +1203,395 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="D6" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="D7" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>56</v>
       </c>
-      <c r="D8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="D8" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="D10" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="D11" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="D12" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="D13" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <v>61</v>
       </c>
-      <c r="D14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="D14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="D16" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="D17" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="D18" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="4">
         <v>17</v>
       </c>
-      <c r="D19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="D19" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="4">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="D20" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="D21" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="4">
         <v>16</v>
       </c>
-      <c r="D22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="D22" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="4">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="35.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="D23" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="35.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="4">
         <v>2</v>
       </c>
-      <c r="D24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="D24" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="4">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="D25" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="4">
         <v>4</v>
       </c>
-      <c r="D26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="D26" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="4">
         <v>4</v>
       </c>
-      <c r="D27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="D27" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="3" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="2">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="35.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="D28" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="35.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="4">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="5" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>